<commit_message>
add api transaction request report (list, create, detail, update, delete by id, delete, preview)
</commit_message>
<xml_diff>
--- a/assets/template/Template Transaction.xlsx
+++ b/assets/template/Template Transaction.xlsx
@@ -10,22 +10,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="G3">
-      <text>
-        <t xml:space="preserve">di isi dengan "Domestik" atau "Ekspor"
-	-paramita deli</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
   <si>
@@ -207,11 +191,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="0.000;[Red]0.000"/>
-    <numFmt numFmtId="165" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00;\(#,##0.00\)"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="mm&quot;-&quot;dd&quot;-&quot;yyyy"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -337,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="30">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -350,31 +332,25 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -384,18 +360,18 @@
     <xf borderId="1" fillId="2" fontId="3" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="3" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="3" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="2" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -404,36 +380,30 @@
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="2" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="6" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="6" fillId="2" fontId="6" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="6" fillId="2" fontId="6" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="6" fillId="2" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="2" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="6" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="6" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="6" fillId="2" fontId="6" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="2" fontId="6" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="7" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="6" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="6" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="2" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -728,32 +698,32 @@
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
+      <c r="P1" s="4"/>
       <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
+      <c r="R1" s="4"/>
       <c r="S1" s="2"/>
-      <c r="T1" s="3"/>
+      <c r="T1" s="4"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
       <c r="AA1" s="5"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="3"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="6"/>
       <c r="AG1" s="5"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="2"/>
-      <c r="AJ1" s="6"/>
+      <c r="AH1" s="6"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="4"/>
       <c r="AK1" s="2"/>
       <c r="AL1" s="2"/>
-      <c r="AM1" s="3"/>
+      <c r="AM1" s="4"/>
       <c r="AN1" s="7"/>
-      <c r="AO1" s="3"/>
+      <c r="AO1" s="4"/>
       <c r="AP1" s="7"/>
       <c r="AQ1" s="7"/>
       <c r="AR1" s="7"/>
@@ -763,186 +733,186 @@
       <c r="AV1" s="7"/>
       <c r="AW1" s="7"/>
       <c r="AX1" s="7"/>
-      <c r="AY1" s="8"/>
-      <c r="AZ1" s="8"/>
+      <c r="AY1" s="5"/>
+      <c r="AZ1" s="5"/>
       <c r="BA1" s="2"/>
-      <c r="BB1" s="3"/>
+      <c r="BB1" s="4"/>
       <c r="BC1" s="2"/>
-      <c r="BD1" s="8"/>
+      <c r="BD1" s="5"/>
       <c r="BE1" s="5"/>
       <c r="BF1" s="2"/>
       <c r="BG1" s="2"/>
-      <c r="BH1" s="9"/>
+      <c r="BH1" s="4"/>
       <c r="BI1" s="2"/>
       <c r="BJ1" s="2"/>
       <c r="BK1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="13" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="13" t="s">
+      <c r="L2" s="12"/>
+      <c r="M2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="14"/>
-      <c r="O2" s="15" t="s">
+      <c r="N2" s="12"/>
+      <c r="O2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="13" t="s">
+      <c r="Q2" s="12"/>
+      <c r="R2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="14"/>
-      <c r="T2" s="16" t="s">
+      <c r="S2" s="12"/>
+      <c r="T2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="14"/>
-      <c r="V2" s="10"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="8"/>
       <c r="W2" s="10"/>
-      <c r="X2" s="17" t="s">
+      <c r="X2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="18"/>
-      <c r="Z2" s="18"/>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="18"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="16" t="s">
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="16"/>
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="AE2" s="18"/>
-      <c r="AF2" s="18"/>
-      <c r="AG2" s="18"/>
-      <c r="AH2" s="18"/>
-      <c r="AI2" s="14"/>
-      <c r="AJ2" s="19" t="s">
+      <c r="AE2" s="16"/>
+      <c r="AF2" s="16"/>
+      <c r="AG2" s="16"/>
+      <c r="AH2" s="16"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="AK2" s="14"/>
-      <c r="AL2" s="10"/>
-      <c r="AM2" s="16" t="s">
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="AN2" s="14"/>
-      <c r="AO2" s="20" t="s">
+      <c r="AN2" s="12"/>
+      <c r="AO2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="AP2" s="14"/>
-      <c r="AQ2" s="16" t="s">
+      <c r="AP2" s="12"/>
+      <c r="AQ2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="AR2" s="18"/>
-      <c r="AS2" s="18"/>
-      <c r="AT2" s="18"/>
-      <c r="AU2" s="18"/>
-      <c r="AV2" s="18"/>
-      <c r="AW2" s="18"/>
-      <c r="AX2" s="18"/>
-      <c r="AY2" s="18"/>
-      <c r="AZ2" s="14"/>
-      <c r="BA2" s="10"/>
-      <c r="BB2" s="16" t="s">
+      <c r="AR2" s="16"/>
+      <c r="AS2" s="16"/>
+      <c r="AT2" s="16"/>
+      <c r="AU2" s="16"/>
+      <c r="AV2" s="16"/>
+      <c r="AW2" s="16"/>
+      <c r="AX2" s="16"/>
+      <c r="AY2" s="16"/>
+      <c r="AZ2" s="12"/>
+      <c r="BA2" s="8"/>
+      <c r="BB2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="BC2" s="18"/>
-      <c r="BD2" s="18"/>
-      <c r="BE2" s="14"/>
-      <c r="BF2" s="10"/>
-      <c r="BG2" s="13" t="s">
+      <c r="BC2" s="16"/>
+      <c r="BD2" s="16"/>
+      <c r="BE2" s="12"/>
+      <c r="BF2" s="8"/>
+      <c r="BG2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="BH2" s="14"/>
-      <c r="BI2" s="13" t="s">
+      <c r="BH2" s="12"/>
+      <c r="BI2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="BJ2" s="18"/>
-      <c r="BK2" s="14"/>
+      <c r="BJ2" s="16"/>
+      <c r="BK2" s="12"/>
     </row>
     <row r="3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="22" t="s">
+      <c r="N3" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="O3" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="P3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="22" t="s">
+      <c r="Q3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="22" t="s">
+      <c r="R3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="S3" s="22" t="s">
+      <c r="S3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="24" t="s">
+      <c r="T3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="U3" s="22" t="s">
+      <c r="U3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="V3" s="22" t="s">
+      <c r="V3" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="W3" s="22" t="s">
+      <c r="W3" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="X3" s="24" t="s">
+      <c r="X3" s="21" t="s">
         <v>31</v>
       </c>
       <c r="Y3" s="25" t="s">
@@ -951,16 +921,16 @@
       <c r="Z3" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="AA3" s="26" t="s">
+      <c r="AA3" s="24" t="s">
         <v>34</v>
       </c>
       <c r="AB3" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="AC3" s="22" t="s">
+      <c r="AC3" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="AD3" s="24" t="s">
+      <c r="AD3" s="21" t="s">
         <v>31</v>
       </c>
       <c r="AE3" s="25" t="s">
@@ -969,119 +939,118 @@
       <c r="AF3" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="AG3" s="26" t="s">
+      <c r="AG3" s="24" t="s">
         <v>34</v>
       </c>
       <c r="AH3" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="AI3" s="22" t="s">
+      <c r="AI3" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="AJ3" s="27" t="s">
+      <c r="AJ3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="AK3" s="22" t="s">
+      <c r="AK3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="AL3" s="28" t="s">
+      <c r="AL3" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="AM3" s="24" t="s">
+      <c r="AM3" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AN3" s="29" t="s">
+      <c r="AN3" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="AO3" s="24" t="s">
+      <c r="AO3" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="AP3" s="29" t="s">
+      <c r="AP3" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="AQ3" s="29" t="s">
+      <c r="AQ3" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="AR3" s="29" t="s">
+      <c r="AR3" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="AS3" s="29" t="s">
+      <c r="AS3" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="AT3" s="29" t="s">
+      <c r="AT3" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="AU3" s="29" t="s">
+      <c r="AU3" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="AV3" s="29" t="s">
+      <c r="AV3" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="AW3" s="29" t="s">
+      <c r="AW3" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="AX3" s="29" t="s">
+      <c r="AX3" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="AY3" s="30" t="s">
+      <c r="AY3" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="AZ3" s="30" t="s">
+      <c r="AZ3" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="BA3" s="31" t="s">
+      <c r="BA3" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="BB3" s="32" t="s">
+      <c r="BB3" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="BC3" s="22" t="s">
+      <c r="BC3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="BD3" s="30" t="s">
+      <c r="BD3" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="BE3" s="26" t="s">
+      <c r="BE3" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="BF3" s="22" t="s">
+      <c r="BF3" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="BG3" s="22" t="s">
+      <c r="BG3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="BH3" s="33" t="s">
+      <c r="BH3" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="BI3" s="22" t="s">
+      <c r="BI3" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="BJ3" s="22" t="s">
+      <c r="BJ3" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="BK3" s="22" t="s">
+      <c r="BK3" s="20" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="X2:AC2"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="BI2:BK2"/>
-    <mergeCell ref="BG2:BH2"/>
+    <mergeCell ref="AD2:AI2"/>
+    <mergeCell ref="AJ2:AK2"/>
     <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="AJ2:AK2"/>
     <mergeCell ref="AO2:AP2"/>
-    <mergeCell ref="AD2:AI2"/>
     <mergeCell ref="AQ2:AZ2"/>
     <mergeCell ref="BB2:BE2"/>
+    <mergeCell ref="BG2:BH2"/>
+    <mergeCell ref="BI2:BK2"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="X2:AC2"/>
   </mergeCells>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>